<commit_message>
new order in plots
</commit_message>
<xml_diff>
--- a/activos.xlsx
+++ b/activos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\COVID-YUCATAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2EAA45-3462-47C1-BA84-A3251C1D310D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A81122-1184-47D4-AFE2-F61418A67B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{0297B9A8-727B-441B-AF0F-97223752A483}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0297B9A8-727B-441B-AF0F-97223752A483}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -394,18 +394,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FDFD31-22FA-4E1C-938F-B8450315D761}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -416,7 +416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>13</v>
       </c>
@@ -427,7 +427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>14</v>
       </c>
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>15</v>
       </c>
@@ -449,7 +449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>16</v>
       </c>
@@ -460,7 +460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>17</v>
       </c>
@@ -471,7 +471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>18</v>
       </c>
@@ -482,7 +482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>19</v>
       </c>
@@ -493,7 +493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>20</v>
       </c>
@@ -504,7 +504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>21</v>
       </c>
@@ -515,7 +515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>22</v>
       </c>
@@ -526,7 +526,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>23</v>
       </c>
@@ -537,7 +537,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>24</v>
       </c>
@@ -548,7 +548,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>25</v>
       </c>
@@ -559,7 +559,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>26</v>
       </c>
@@ -570,7 +570,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>27</v>
       </c>
@@ -581,7 +581,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>28</v>
       </c>
@@ -592,7 +592,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>29</v>
       </c>
@@ -603,7 +603,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>30</v>
       </c>
@@ -614,7 +614,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>31</v>
       </c>
@@ -625,7 +625,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -636,7 +636,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -647,7 +647,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -658,7 +658,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
@@ -669,7 +669,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -680,7 +680,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
@@ -691,7 +691,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -702,7 +702,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>8</v>
       </c>
@@ -713,7 +713,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>9</v>
       </c>
@@ -724,7 +724,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10</v>
       </c>
@@ -735,7 +735,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>11</v>
       </c>
@@ -746,7 +746,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>12</v>
       </c>
@@ -757,7 +757,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>13</v>
       </c>
@@ -768,7 +768,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>14</v>
       </c>
@@ -779,7 +779,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>15</v>
       </c>
@@ -790,7 +790,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>16</v>
       </c>
@@ -801,7 +801,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>17</v>
       </c>
@@ -812,7 +812,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>18</v>
       </c>
@@ -823,7 +823,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>19</v>
       </c>
@@ -834,7 +834,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>20</v>
       </c>
@@ -845,7 +845,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>21</v>
       </c>
@@ -856,7 +856,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>22</v>
       </c>
@@ -867,7 +867,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>23</v>
       </c>
@@ -878,7 +878,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>24</v>
       </c>
@@ -889,7 +889,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>25</v>
       </c>
@@ -900,7 +900,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>26</v>
       </c>
@@ -911,7 +911,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>27</v>
       </c>
@@ -922,7 +922,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>28</v>
       </c>
@@ -933,7 +933,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>29</v>
       </c>
@@ -944,7 +944,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>30</v>
       </c>
@@ -955,7 +955,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1</v>
       </c>
@@ -966,7 +966,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2</v>
       </c>
@@ -977,7 +977,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>3</v>
       </c>
@@ -988,7 +988,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>4</v>
       </c>
@@ -999,7 +999,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>5</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>6</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>7</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>8</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>9</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>10</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>11</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>12</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>13</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>14</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>15</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>16</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>17</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>18</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>19</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>20</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>21</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>22</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>23</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>24</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>25</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>26</v>
       </c>
@@ -1239,6 +1239,17 @@
       </c>
       <c r="C76">
         <v>1581</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>27</v>
+      </c>
+      <c r="B77">
+        <v>329</v>
+      </c>
+      <c r="C77">
+        <v>1616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update db and models
</commit_message>
<xml_diff>
--- a/activos.xlsx
+++ b/activos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\COVID-YUCATAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DBB4CE-EB79-4ECA-8CE4-CC303E5E791C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FE2304-0856-49B4-B959-08E5297308F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -309,7 +309,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136:B139"/>
+      <selection activeCell="B140" sqref="B140:B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1848,8 +1848,28 @@
         <v>9083</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>29</v>
+      </c>
+      <c r="B140">
+        <v>906</v>
+      </c>
+      <c r="C140">
+        <v>9283</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>30</v>
+      </c>
+      <c r="B141">
+        <v>937</v>
+      </c>
+      <c r="C141">
+        <v>9527</v>
+      </c>
+    </row>
     <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update database and create backup file
</commit_message>
<xml_diff>
--- a/activos.xlsx
+++ b/activos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\COVID-YUCATAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\repositorios\COVID-YUCATAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A0922-0154-4C23-A76F-DE96CEE3C7BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1351EB62-1CE8-4356-9AF8-074436E23CCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -308,18 +308,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="C195" sqref="C195"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="C197" sqref="C197"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.58203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.3984375" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" customWidth="1"/>
-    <col min="4" max="26" width="9.3984375" customWidth="1"/>
+    <col min="1" max="2" width="9.4140625" customWidth="1"/>
+    <col min="3" max="3" width="16.58203125" customWidth="1"/>
+    <col min="4" max="26" width="9.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -330,7 +330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>13</v>
       </c>
@@ -341,7 +341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>14</v>
       </c>
@@ -352,7 +352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>15</v>
       </c>
@@ -363,7 +363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>16</v>
       </c>
@@ -374,7 +374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>17</v>
       </c>
@@ -385,7 +385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>18</v>
       </c>
@@ -396,7 +396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>19</v>
       </c>
@@ -407,7 +407,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>20</v>
       </c>
@@ -418,7 +418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>21</v>
       </c>
@@ -429,7 +429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>22</v>
       </c>
@@ -440,7 +440,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>23</v>
       </c>
@@ -451,7 +451,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>24</v>
       </c>
@@ -462,7 +462,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>25</v>
       </c>
@@ -473,7 +473,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>26</v>
       </c>
@@ -484,7 +484,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>27</v>
       </c>
@@ -495,7 +495,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>28</v>
       </c>
@@ -506,7 +506,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>29</v>
       </c>
@@ -517,7 +517,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>30</v>
       </c>
@@ -528,7 +528,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>31</v>
       </c>
@@ -539,7 +539,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -550,7 +550,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -561,7 +561,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -572,7 +572,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -583,7 +583,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -594,7 +594,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>6</v>
       </c>
@@ -605,7 +605,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>7</v>
       </c>
@@ -616,7 +616,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>8</v>
       </c>
@@ -627,7 +627,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>9</v>
       </c>
@@ -638,7 +638,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>10</v>
       </c>
@@ -649,7 +649,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>11</v>
       </c>
@@ -660,7 +660,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>12</v>
       </c>
@@ -671,7 +671,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>13</v>
       </c>
@@ -682,7 +682,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>14</v>
       </c>
@@ -693,7 +693,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>15</v>
       </c>
@@ -704,7 +704,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>16</v>
       </c>
@@ -715,7 +715,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>17</v>
       </c>
@@ -726,7 +726,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>18</v>
       </c>
@@ -737,7 +737,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>19</v>
       </c>
@@ -748,7 +748,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>20</v>
       </c>
@@ -759,7 +759,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>21</v>
       </c>
@@ -770,7 +770,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>22</v>
       </c>
@@ -781,7 +781,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>23</v>
       </c>
@@ -792,7 +792,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>24</v>
       </c>
@@ -803,7 +803,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>25</v>
       </c>
@@ -814,7 +814,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>26</v>
       </c>
@@ -825,7 +825,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>27</v>
       </c>
@@ -836,7 +836,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>28</v>
       </c>
@@ -847,7 +847,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>29</v>
       </c>
@@ -858,7 +858,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>30</v>
       </c>
@@ -869,7 +869,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>1</v>
       </c>
@@ -880,7 +880,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>2</v>
       </c>
@@ -891,7 +891,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>3</v>
       </c>
@@ -902,7 +902,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>4</v>
       </c>
@@ -913,7 +913,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>5</v>
       </c>
@@ -924,7 +924,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>6</v>
       </c>
@@ -935,7 +935,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>7</v>
       </c>
@@ -946,7 +946,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>8</v>
       </c>
@@ -957,7 +957,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>9</v>
       </c>
@@ -968,7 +968,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>10</v>
       </c>
@@ -979,7 +979,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>11</v>
       </c>
@@ -990,7 +990,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>12</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>13</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>14</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>15</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>16</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>17</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>18</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>19</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>20</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>21</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>22</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>23</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>24</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>25</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>26</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>27</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>28</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>1675</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>29</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>30</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>31</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>1</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>2</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>1933</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>3</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>4</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>5</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>6</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>2116</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>7</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>2146</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>8</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>2167</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>9</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>10</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>2299</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>11</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>2357</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>12</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>13</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>2488</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>14</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>2544</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>15</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>16</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>2665</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>17</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>2741</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>18</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>19</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>20</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>3006</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>21</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>3096</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>22</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>3191</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>23</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>3351</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>24</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>3554</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>25</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>26</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>3841</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="4">
         <v>27</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>4018</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="4">
         <v>28</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>4177</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="4">
         <v>29</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>4265</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="4">
         <v>30</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>4441</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="4">
         <v>1</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>4549</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="4">
         <v>2</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>4631</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="4">
         <v>3</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>4886</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="4">
         <v>4</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>5011</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="4">
         <v>5</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>5110</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="4">
         <v>6</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>5259</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="4">
         <v>7</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>5415</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>8</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>5580</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>9</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>5739</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>10</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>5926</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>11</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>6117</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>12</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>6276</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>13</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>6385</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>14</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>6661</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>15</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>6826</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>16</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>6954</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>17</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>7073</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>18</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>7165</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>19</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>7358</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>20</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>7475</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>21</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>7576</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>22</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>7813</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>23</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>8062</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>24</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>8322</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>25</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>8503</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>26</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>8729</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>27</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>8881</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>28</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>9083</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>29</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>9283</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>30</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>9527</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>31</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>9767</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>1</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>10223</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>2</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>10438</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>3</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>10575</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>4</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>10743</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>5</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>10922</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>6</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>11170</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>7</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>11337</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>8</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>11541</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>9</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>11643</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>10</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>11822</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>11</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>12033</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>12</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>12131</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>13</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>12289</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>14</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>12440</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>15</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>12539</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>16</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>12708</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>17</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>12818</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>18</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>12963</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>19</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>13125</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>20</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>13352</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>21</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>13492</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>22</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>13664</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>23</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>13743</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>24</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>13853</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>25</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>14041</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>26</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>14208</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>27</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>14373</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>28</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>14475</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>29</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>14705</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>30</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>14832</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>31</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>14928</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>1</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>15085</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>2</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>15236</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>3</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>15425</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>4</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>15551</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>5</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>15743</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>6</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>15828</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>7</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>15932</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>8</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>16051</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>9</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>16179</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>10</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>16355</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>11</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>16538</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>12</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>16619</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>13</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>16831</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>14</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>16895</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>15</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>16982</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>16</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>17061</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>17</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>17142</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>18</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>17242</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>19</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>17390</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>20</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>17474</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>21</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>17539</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>22</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>17649</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>23</v>
       </c>
@@ -2475,810 +2475,860 @@
         <v>17714</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>24</v>
+      </c>
+      <c r="B197">
+        <v>921</v>
+      </c>
+      <c r="C197">
+        <v>17855</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>25</v>
+      </c>
+      <c r="B198">
+        <v>936</v>
+      </c>
+      <c r="C198">
+        <v>17968</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>26</v>
+      </c>
+      <c r="B199">
+        <v>975</v>
+      </c>
+      <c r="C199">
+        <v>18115</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>27</v>
+      </c>
+      <c r="B200">
+        <v>969</v>
+      </c>
+      <c r="C200">
+        <v>18215</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>28</v>
+      </c>
+      <c r="B201">
+        <v>1009</v>
+      </c>
+      <c r="C201">
+        <v>18325</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update data models and national cases
</commit_message>
<xml_diff>
--- a/activos.xlsx
+++ b/activos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\repositorios\COVID-YUCATAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1351EB62-1CE8-4356-9AF8-074436E23CCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564E0BE1-1B2C-4CAD-82BC-1F0427235571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2120" yWindow="2120" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -309,7 +309,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.58203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2530,9 +2530,39 @@
         <v>18325</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>29</v>
+      </c>
+      <c r="B202">
+        <v>1034</v>
+      </c>
+      <c r="C202">
+        <v>18403</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>30</v>
+      </c>
+      <c r="B203">
+        <v>1014</v>
+      </c>
+      <c r="C203">
+        <v>18511</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>1</v>
+      </c>
+      <c r="B204">
+        <v>1033</v>
+      </c>
+      <c r="C204">
+        <v>18628</v>
+      </c>
+    </row>
     <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update local and national database
</commit_message>
<xml_diff>
--- a/activos.xlsx
+++ b/activos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\repositorios\COVID-YUCATAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564E0BE1-1B2C-4CAD-82BC-1F0427235571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEF23B2-880D-445F-95FF-4DEC10BC80D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="2120" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -308,8 +308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="C200" sqref="C200"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="C205" sqref="C205:C209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.58203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2563,26 +2563,76 @@
         <v>18628</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>2</v>
+      </c>
+      <c r="B205">
+        <v>1044</v>
+      </c>
+      <c r="C205">
+        <v>18734</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>3</v>
+      </c>
+      <c r="B206">
+        <v>1044</v>
+      </c>
+      <c r="C206">
+        <v>18837</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>4</v>
+      </c>
+      <c r="B207">
+        <v>1074</v>
+      </c>
+      <c r="C207">
+        <v>18958</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>5</v>
+      </c>
+      <c r="B208">
+        <v>1049</v>
+      </c>
+      <c r="C208">
+        <v>19019</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>6</v>
+      </c>
+      <c r="B209">
+        <v>955</v>
+      </c>
+      <c r="C209">
+        <v>19070</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update database and models
</commit_message>
<xml_diff>
--- a/activos.xlsx
+++ b/activos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\repositorios\COVID-YUCATAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEF23B2-880D-445F-95FF-4DEC10BC80D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4945D3EC-DA70-4622-8969-8367DE41675F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -309,17 +309,17 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="C205" sqref="C205:C209"/>
+      <selection activeCell="C210" sqref="C210:C212"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.58203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.4140625" customWidth="1"/>
-    <col min="3" max="3" width="16.58203125" customWidth="1"/>
-    <col min="4" max="26" width="9.4140625" customWidth="1"/>
+    <col min="1" max="2" width="9.375" customWidth="1"/>
+    <col min="3" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="26" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -330,7 +330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>13</v>
       </c>
@@ -341,7 +341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>14</v>
       </c>
@@ -352,7 +352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>15</v>
       </c>
@@ -363,7 +363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>16</v>
       </c>
@@ -374,7 +374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>17</v>
       </c>
@@ -385,7 +385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>18</v>
       </c>
@@ -396,7 +396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>19</v>
       </c>
@@ -407,7 +407,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>20</v>
       </c>
@@ -418,7 +418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>21</v>
       </c>
@@ -429,7 +429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>22</v>
       </c>
@@ -440,7 +440,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>23</v>
       </c>
@@ -451,7 +451,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>24</v>
       </c>
@@ -462,7 +462,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>25</v>
       </c>
@@ -473,7 +473,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>26</v>
       </c>
@@ -484,7 +484,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>27</v>
       </c>
@@ -495,7 +495,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>28</v>
       </c>
@@ -506,7 +506,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>29</v>
       </c>
@@ -517,7 +517,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>30</v>
       </c>
@@ -528,7 +528,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>31</v>
       </c>
@@ -539,7 +539,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -550,7 +550,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -561,7 +561,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -572,7 +572,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -583,7 +583,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -594,7 +594,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>6</v>
       </c>
@@ -605,7 +605,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>7</v>
       </c>
@@ -616,7 +616,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>8</v>
       </c>
@@ -627,7 +627,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>9</v>
       </c>
@@ -638,7 +638,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>10</v>
       </c>
@@ -649,7 +649,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>11</v>
       </c>
@@ -660,7 +660,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>12</v>
       </c>
@@ -671,7 +671,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>13</v>
       </c>
@@ -682,7 +682,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>14</v>
       </c>
@@ -693,7 +693,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>15</v>
       </c>
@@ -704,7 +704,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>16</v>
       </c>
@@ -715,7 +715,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>17</v>
       </c>
@@ -726,7 +726,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>18</v>
       </c>
@@ -737,7 +737,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>19</v>
       </c>
@@ -748,7 +748,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>20</v>
       </c>
@@ -759,7 +759,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>21</v>
       </c>
@@ -770,7 +770,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>22</v>
       </c>
@@ -781,7 +781,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>23</v>
       </c>
@@ -792,7 +792,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>24</v>
       </c>
@@ -803,7 +803,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>25</v>
       </c>
@@ -814,7 +814,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>26</v>
       </c>
@@ -825,7 +825,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>27</v>
       </c>
@@ -836,7 +836,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>28</v>
       </c>
@@ -847,7 +847,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>29</v>
       </c>
@@ -858,7 +858,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>30</v>
       </c>
@@ -869,7 +869,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>1</v>
       </c>
@@ -880,7 +880,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>2</v>
       </c>
@@ -891,7 +891,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>3</v>
       </c>
@@ -902,7 +902,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>4</v>
       </c>
@@ -913,7 +913,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>5</v>
       </c>
@@ -924,7 +924,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>6</v>
       </c>
@@ -935,7 +935,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>7</v>
       </c>
@@ -946,7 +946,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>8</v>
       </c>
@@ -957,7 +957,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>9</v>
       </c>
@@ -968,7 +968,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>10</v>
       </c>
@@ -979,7 +979,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>11</v>
       </c>
@@ -990,7 +990,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>12</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>13</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>14</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>15</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>16</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>17</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>18</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>19</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>20</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>21</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>22</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>23</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>24</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>25</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>26</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>27</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>28</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>1675</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>29</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>30</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>31</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>1</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>2</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>1933</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>3</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>4</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>5</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>6</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>2116</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>7</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>2146</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>8</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>2167</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>9</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>10</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>2299</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>11</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>2357</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>12</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>13</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>2488</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>14</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>2544</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>15</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>16</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>2665</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>17</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>2741</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>18</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>19</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>20</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>3006</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>21</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>3096</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>22</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>3191</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>23</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>3351</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>24</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>3554</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>25</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>26</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>3841</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>27</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>4018</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>28</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>4177</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>29</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>4265</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>30</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>4441</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>1</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>4549</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>2</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>4631</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>3</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>4886</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>4</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>5011</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>5</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>5110</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>6</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>5259</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>7</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>5415</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>8</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>5580</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>9</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>5739</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>10</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>5926</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>11</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>6117</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>12</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>6276</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>13</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>6385</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>14</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>6661</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>15</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>6826</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>16</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>6954</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>17</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>7073</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>18</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>7165</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>19</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>7358</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>20</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>7475</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>21</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>7576</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>22</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>7813</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>23</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>8062</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>24</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>8322</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>25</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>8503</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>26</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>8729</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>27</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>8881</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>28</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>9083</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>29</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>9283</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>30</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>9527</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>31</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>9767</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>1</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>10223</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>2</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>10438</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>3</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>10575</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>4</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>10743</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>5</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>10922</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>6</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>11170</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>7</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>11337</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>8</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>11541</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>9</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>11643</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>10</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>11822</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>11</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>12033</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>12</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>12131</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>13</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>12289</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>14</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>12440</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>15</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>12539</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>16</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>12708</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>17</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>12818</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>18</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>12963</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>19</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>13125</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>20</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>13352</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>21</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>13492</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>22</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>13664</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>23</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>13743</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>24</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>13853</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>25</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>14041</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>26</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>14208</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>27</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>14373</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>28</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>14475</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>29</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>14705</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>30</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>14832</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>31</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>14928</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>1</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>15085</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>2</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>15236</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>3</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>15425</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>4</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>15551</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>5</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>15743</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>6</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>15828</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>7</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>15932</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>8</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>16051</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>9</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>16179</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>10</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>16355</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>11</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>16538</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>12</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>16619</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>13</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>16831</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>14</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>16895</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>15</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>16982</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>16</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>17061</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>17</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>17142</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>18</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>17242</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>19</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>17390</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>20</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>17474</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>21</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>17539</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>22</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>17649</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>23</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>17714</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>24</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>17855</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>25</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>17968</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>26</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>18115</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>27</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>18215</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>28</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>18325</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>29</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>18403</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>30</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>18511</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>1</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>18628</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>2</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>18734</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>3</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>18837</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>4</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>18958</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>5</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>19019</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>6</v>
       </c>
@@ -2618,797 +2618,827 @@
         <v>19070</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>7</v>
+      </c>
+      <c r="B210">
+        <v>951</v>
+      </c>
+      <c r="C210">
+        <v>19110</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>8</v>
+      </c>
+      <c r="B211">
+        <v>903</v>
+      </c>
+      <c r="C211">
+        <v>19208</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>9</v>
+      </c>
+      <c r="B212">
+        <v>890</v>
+      </c>
+      <c r="C212">
+        <v>19308</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>